<commit_message>
Auto update stock data
</commit_message>
<xml_diff>
--- a/Stock_Risk_Scores.xlsx
+++ b/Stock_Risk_Scores.xlsx
@@ -490,7 +490,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Current Oct 25 Oct 22, 2025</t>
+          <t>Current Oct 25 Oct 23, 2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -837,7 +837,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Current Oct 25 Oct 22, 2025</t>
+          <t>Current Oct 25 Oct 23, 2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1188,12 +1188,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Current Oct 25 Oct 22, 2025</t>
+          <t>Current Oct 25 Oct 23, 2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>12.24</t>
+          <t>12.19</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -1539,12 +1539,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Current Oct 25 Oct 22, 2025</t>
+          <t>Current Oct 25 Oct 23, 2025</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8.88</t>
+          <t>8.89</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">

</xml_diff>